<commit_message>
Change hierarchy of Reports and update Vplan template
Signed-off-by: MikeOpenHWGroup <mike@openhwgroup.org>
</commit_message>
<xml_diff>
--- a/docs/VerifPlans/templates/CORE-V_Simulation_VerifPlan_Template.xlsx
+++ b/docs/VerifPlans/templates/CORE-V_Simulation_VerifPlan_Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t xml:space="preserve">Requirement Location</t>
   </si>
@@ -72,7 +72,7 @@
     <t xml:space="preserve">Functional Coverage</t>
   </si>
   <si>
-    <t xml:space="preserve">Check against ISS</t>
+    <t xml:space="preserve">Check against RM</t>
   </si>
   <si>
     <t xml:space="preserve">Directed Self-Checking</t>
@@ -81,7 +81,7 @@
     <t xml:space="preserve">Assertion Coverage</t>
   </si>
   <si>
-    <t xml:space="preserve">Check against RM</t>
+    <t xml:space="preserve">Assertion Check</t>
   </si>
   <si>
     <t xml:space="preserve">Directed Non-Self-Checking</t>
@@ -90,7 +90,7 @@
     <t xml:space="preserve">Code Coverage</t>
   </si>
   <si>
-    <t xml:space="preserve">Assertion Check</t>
+    <t xml:space="preserve">Any/All</t>
   </si>
   <si>
     <t xml:space="preserve">Constrained-Random</t>
@@ -99,13 +99,10 @@
     <t xml:space="preserve">N/A</t>
   </si>
   <si>
-    <t xml:space="preserve">Any/All</t>
+    <t xml:space="preserve">Other</t>
   </si>
   <si>
     <t xml:space="preserve">ENV capability, not specific test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
   </si>
   <si>
     <t xml:space="preserve">Reference Name</t>
@@ -379,7 +376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -388,10 +385,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="17.0078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.3"/>
@@ -1379,14 +1376,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1431,7 +1428,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>16</v>
       </c>
@@ -1442,7 +1439,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>19</v>
       </c>
@@ -1453,7 +1450,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>22</v>
       </c>
@@ -1474,16 +1471,13 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="C10" s="0" t="s">
         <v>24</v>
       </c>
@@ -1500,7 +1494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1510,7 +1504,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.57421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.32"/>
@@ -1521,41 +1515,41 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>